<commit_message>
Added support for privacy settings
</commit_message>
<xml_diff>
--- a/data/to-migrate/mapping/Professional Actitivies Choice Lists.xlsx
+++ b/data/to-migrate/mapping/Professional Actitivies Choice Lists.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsmith/Documents/code/lyterati-elements/data/to-migrate/mapping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC88C261-DD0F-C248-AC7C-05B4D8A1755E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8126C662-63A1-5746-AAFE-806DEAF23D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" xr2:uid="{981C8887-6331-42CE-8691-63AB4AAAF8BA}"/>
   </bookViews>
@@ -56,7 +56,7 @@
     <t>Non-Government Organization</t>
   </si>
   <si>
-    <t>c-membership-type</t>
+    <t>Elements</t>
   </si>
 </sst>
 </file>
@@ -431,7 +431,7 @@
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection sqref="A1:A7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>